<commit_message>
Update classifier figures so that y-axis is assigned probablity of TB susceptibility.
Also update supp data S5 to report assigned probability of TB susceptibility.
</commit_message>
<xml_diff>
--- a/data/Supplementary_Data_S5.xlsx
+++ b/data/Supplementary_Data_S5.xlsx
@@ -1617,7 +1617,7 @@
     <t>r19-resist-noninf</t>
   </si>
   <si>
-    <t>prob_tb_resist</t>
+    <t>prob_tb_suscep</t>
   </si>
   <si>
     <t>u02-unknow-noninf</t>
@@ -11398,7 +11398,7 @@
         <v>510</v>
       </c>
       <c r="C2" t="n">
-        <v>0.643889583596928</v>
+        <v>0.356110416403072</v>
       </c>
     </row>
     <row r="3">
@@ -11409,7 +11409,7 @@
         <v>510</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0222923220765249</v>
+        <v>0.977707677923475</v>
       </c>
     </row>
     <row r="4">
@@ -11420,7 +11420,7 @@
         <v>510</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0602875285371711</v>
+        <v>0.939712471462829</v>
       </c>
     </row>
     <row r="5">
@@ -11431,7 +11431,7 @@
         <v>510</v>
       </c>
       <c r="C5" t="n">
-        <v>0.582875698433411</v>
+        <v>0.417124301566589</v>
       </c>
     </row>
     <row r="6">
@@ -11442,7 +11442,7 @@
         <v>510</v>
       </c>
       <c r="C6" t="n">
-        <v>0.644659328166742</v>
+        <v>0.355340671833258</v>
       </c>
     </row>
     <row r="7">
@@ -11453,7 +11453,7 @@
         <v>516</v>
       </c>
       <c r="C7" t="n">
-        <v>0.977119898190868</v>
+        <v>0.0228801018091317</v>
       </c>
     </row>
     <row r="8">
@@ -11464,7 +11464,7 @@
         <v>516</v>
       </c>
       <c r="C8" t="n">
-        <v>0.969311998286482</v>
+        <v>0.0306880017135178</v>
       </c>
     </row>
     <row r="9">
@@ -11475,7 +11475,7 @@
         <v>516</v>
       </c>
       <c r="C9" t="n">
-        <v>0.988435451273617</v>
+        <v>0.0115645487263826</v>
       </c>
     </row>
     <row r="10">
@@ -11486,7 +11486,7 @@
         <v>516</v>
       </c>
       <c r="C10" t="n">
-        <v>0.97592097279484</v>
+        <v>0.0240790272051596</v>
       </c>
     </row>
     <row r="11">
@@ -11497,7 +11497,7 @@
         <v>516</v>
       </c>
       <c r="C11" t="n">
-        <v>0.800279772166368</v>
+        <v>0.199720227833632</v>
       </c>
     </row>
     <row r="12">
@@ -11508,7 +11508,7 @@
         <v>516</v>
       </c>
       <c r="C12" t="n">
-        <v>0.826209758987449</v>
+        <v>0.173790241012551</v>
       </c>
     </row>
     <row r="13">
@@ -11519,7 +11519,7 @@
         <v>516</v>
       </c>
       <c r="C13" t="n">
-        <v>0.950769411316772</v>
+        <v>0.0492305886832276</v>
       </c>
     </row>
     <row r="14">
@@ -11530,7 +11530,7 @@
         <v>516</v>
       </c>
       <c r="C14" t="n">
-        <v>0.854746070186155</v>
+        <v>0.145253929813845</v>
       </c>
     </row>
     <row r="15">
@@ -11541,7 +11541,7 @@
         <v>516</v>
       </c>
       <c r="C15" t="n">
-        <v>0.990028345884766</v>
+        <v>0.00997165411523371</v>
       </c>
     </row>
     <row r="16">
@@ -11552,7 +11552,7 @@
         <v>516</v>
       </c>
       <c r="C16" t="n">
-        <v>0.984645026254381</v>
+        <v>0.0153549737456191</v>
       </c>
     </row>
     <row r="17">
@@ -11563,7 +11563,7 @@
         <v>516</v>
       </c>
       <c r="C17" t="n">
-        <v>0.912962750492624</v>
+        <v>0.0870372495073758</v>
       </c>
     </row>
     <row r="18">
@@ -11574,7 +11574,7 @@
         <v>516</v>
       </c>
       <c r="C18" t="n">
-        <v>0.955604040416059</v>
+        <v>0.0443959595839408</v>
       </c>
     </row>
     <row r="19">
@@ -11585,7 +11585,7 @@
         <v>516</v>
       </c>
       <c r="C19" t="n">
-        <v>0.939147452222853</v>
+        <v>0.0608525477771465</v>
       </c>
     </row>
     <row r="20">
@@ -11596,7 +11596,7 @@
         <v>516</v>
       </c>
       <c r="C20" t="n">
-        <v>0.62099419362789</v>
+        <v>0.37900580637211</v>
       </c>
     </row>
     <row r="21">
@@ -11607,7 +11607,7 @@
         <v>516</v>
       </c>
       <c r="C21" t="n">
-        <v>0.781010351659347</v>
+        <v>0.218989648340653</v>
       </c>
     </row>
     <row r="22">
@@ -11618,7 +11618,7 @@
         <v>516</v>
       </c>
       <c r="C22" t="n">
-        <v>0.55510592843062</v>
+        <v>0.44489407156938</v>
       </c>
     </row>
     <row r="23">
@@ -11629,7 +11629,7 @@
         <v>516</v>
       </c>
       <c r="C23" t="n">
-        <v>0.948493788998948</v>
+        <v>0.051506211001052</v>
       </c>
     </row>
   </sheetData>
@@ -31605,7 +31605,7 @@
         <v>534</v>
       </c>
       <c r="B2" t="n">
-        <v>0.965912837448595</v>
+        <v>0.0340871625514053</v>
       </c>
     </row>
     <row r="3">
@@ -31613,7 +31613,7 @@
         <v>535</v>
       </c>
       <c r="B3" t="n">
-        <v>0.981561455399339</v>
+        <v>0.0184385446006613</v>
       </c>
     </row>
     <row r="4">
@@ -31621,7 +31621,7 @@
         <v>536</v>
       </c>
       <c r="B4" t="n">
-        <v>0.863472555790834</v>
+        <v>0.136527444209166</v>
       </c>
     </row>
     <row r="5">
@@ -31629,7 +31629,7 @@
         <v>537</v>
       </c>
       <c r="B5" t="n">
-        <v>0.996139267646749</v>
+        <v>0.00386073235325146</v>
       </c>
     </row>
     <row r="6">
@@ -31637,7 +31637,7 @@
         <v>538</v>
       </c>
       <c r="B6" t="n">
-        <v>0.869127451037091</v>
+        <v>0.130872548962909</v>
       </c>
     </row>
     <row r="7">
@@ -31645,7 +31645,7 @@
         <v>539</v>
       </c>
       <c r="B7" t="n">
-        <v>0.971684905315139</v>
+        <v>0.028315094684861</v>
       </c>
     </row>
     <row r="8">
@@ -31653,7 +31653,7 @@
         <v>540</v>
       </c>
       <c r="B8" t="n">
-        <v>0.96080628351739</v>
+        <v>0.0391937164826102</v>
       </c>
     </row>
     <row r="9">
@@ -31661,7 +31661,7 @@
         <v>541</v>
       </c>
       <c r="B9" t="n">
-        <v>0.99124944763481</v>
+        <v>0.00875055236519018</v>
       </c>
     </row>
     <row r="10">
@@ -31669,7 +31669,7 @@
         <v>542</v>
       </c>
       <c r="B10" t="n">
-        <v>0.56155934515434</v>
+        <v>0.43844065484566</v>
       </c>
     </row>
     <row r="11">
@@ -31677,7 +31677,7 @@
         <v>543</v>
       </c>
       <c r="B11" t="n">
-        <v>0.848383240189307</v>
+        <v>0.151616759810693</v>
       </c>
     </row>
     <row r="12">
@@ -31685,7 +31685,7 @@
         <v>544</v>
       </c>
       <c r="B12" t="n">
-        <v>0.898565409529099</v>
+        <v>0.101434590470901</v>
       </c>
     </row>
     <row r="13">
@@ -31693,7 +31693,7 @@
         <v>545</v>
       </c>
       <c r="B13" t="n">
-        <v>0.972734970234417</v>
+        <v>0.0272650297655834</v>
       </c>
     </row>
     <row r="14">
@@ -31701,7 +31701,7 @@
         <v>546</v>
       </c>
       <c r="B14" t="n">
-        <v>0.940986913466712</v>
+        <v>0.0590130865332879</v>
       </c>
     </row>
     <row r="15">
@@ -31709,7 +31709,7 @@
         <v>547</v>
       </c>
       <c r="B15" t="n">
-        <v>0.984892059062416</v>
+        <v>0.0151079409375843</v>
       </c>
     </row>
     <row r="16">
@@ -31717,7 +31717,7 @@
         <v>548</v>
       </c>
       <c r="B16" t="n">
-        <v>0.935809484680453</v>
+        <v>0.0641905153195472</v>
       </c>
     </row>
     <row r="17">
@@ -31725,7 +31725,7 @@
         <v>549</v>
       </c>
       <c r="B17" t="n">
-        <v>0.933484680985631</v>
+        <v>0.0665153190143686</v>
       </c>
     </row>
     <row r="18">
@@ -31733,7 +31733,7 @@
         <v>550</v>
       </c>
       <c r="B18" t="n">
-        <v>0.701708704604018</v>
+        <v>0.298291295395982</v>
       </c>
     </row>
     <row r="19">
@@ -31741,7 +31741,7 @@
         <v>551</v>
       </c>
       <c r="B19" t="n">
-        <v>0.977193053292118</v>
+        <v>0.0228069467078816</v>
       </c>
     </row>
     <row r="20">
@@ -31749,7 +31749,7 @@
         <v>552</v>
       </c>
       <c r="B20" t="n">
-        <v>0.977835757662705</v>
+        <v>0.0221642423372947</v>
       </c>
     </row>
     <row r="21">
@@ -31757,7 +31757,7 @@
         <v>553</v>
       </c>
       <c r="B21" t="n">
-        <v>0.893957535226737</v>
+        <v>0.106042464773263</v>
       </c>
     </row>
     <row r="22">
@@ -31765,7 +31765,7 @@
         <v>554</v>
       </c>
       <c r="B22" t="n">
-        <v>0.954215800562905</v>
+        <v>0.0457841994370946</v>
       </c>
     </row>
     <row r="23">
@@ -31773,7 +31773,7 @@
         <v>555</v>
       </c>
       <c r="B23" t="n">
-        <v>0.967983499211579</v>
+        <v>0.0320165007884214</v>
       </c>
     </row>
     <row r="24">
@@ -31781,7 +31781,7 @@
         <v>556</v>
       </c>
       <c r="B24" t="n">
-        <v>0.844132587139272</v>
+        <v>0.155867412860728</v>
       </c>
     </row>
     <row r="25">
@@ -31789,7 +31789,7 @@
         <v>557</v>
       </c>
       <c r="B25" t="n">
-        <v>0.929248140221486</v>
+        <v>0.0707518597785142</v>
       </c>
     </row>
     <row r="26">
@@ -31797,7 +31797,7 @@
         <v>558</v>
       </c>
       <c r="B26" t="n">
-        <v>0.979433743043595</v>
+        <v>0.0205662569564052</v>
       </c>
     </row>
     <row r="27">
@@ -31805,7 +31805,7 @@
         <v>559</v>
       </c>
       <c r="B27" t="n">
-        <v>0.948822754807518</v>
+        <v>0.0511772451924825</v>
       </c>
     </row>
     <row r="28">
@@ -31813,7 +31813,7 @@
         <v>560</v>
       </c>
       <c r="B28" t="n">
-        <v>0.93681235789346</v>
+        <v>0.0631876421065398</v>
       </c>
     </row>
     <row r="29">
@@ -31821,7 +31821,7 @@
         <v>561</v>
       </c>
       <c r="B29" t="n">
-        <v>0.97081074133156</v>
+        <v>0.0291892586684398</v>
       </c>
     </row>
     <row r="30">
@@ -31829,7 +31829,7 @@
         <v>562</v>
       </c>
       <c r="B30" t="n">
-        <v>0.993955400308641</v>
+        <v>0.00604459969135862</v>
       </c>
     </row>
     <row r="31">
@@ -31837,7 +31837,7 @@
         <v>563</v>
       </c>
       <c r="B31" t="n">
-        <v>0.99162758381724</v>
+        <v>0.00837241618275986</v>
       </c>
     </row>
     <row r="32">
@@ -31845,7 +31845,7 @@
         <v>564</v>
       </c>
       <c r="B32" t="n">
-        <v>0.954778082317498</v>
+        <v>0.0452219176825022</v>
       </c>
     </row>
     <row r="33">
@@ -31853,7 +31853,7 @@
         <v>565</v>
       </c>
       <c r="B33" t="n">
-        <v>0.982156355510989</v>
+        <v>0.017843644489011</v>
       </c>
     </row>
     <row r="34">
@@ -31861,7 +31861,7 @@
         <v>566</v>
       </c>
       <c r="B34" t="n">
-        <v>0.906921403225155</v>
+        <v>0.0930785967748445</v>
       </c>
     </row>
     <row r="35">
@@ -31869,7 +31869,7 @@
         <v>567</v>
       </c>
       <c r="B35" t="n">
-        <v>0.78793787886369</v>
+        <v>0.21206212113631</v>
       </c>
     </row>
     <row r="36">
@@ -31877,7 +31877,7 @@
         <v>568</v>
       </c>
       <c r="B36" t="n">
-        <v>0.895193202721991</v>
+        <v>0.104806797278009</v>
       </c>
     </row>
     <row r="37">
@@ -31885,7 +31885,7 @@
         <v>569</v>
       </c>
       <c r="B37" t="n">
-        <v>0.560836858881839</v>
+        <v>0.439163141118161</v>
       </c>
     </row>
     <row r="38">
@@ -31893,7 +31893,7 @@
         <v>570</v>
       </c>
       <c r="B38" t="n">
-        <v>0.740732970023262</v>
+        <v>0.259267029976738</v>
       </c>
     </row>
     <row r="39">
@@ -31901,7 +31901,7 @@
         <v>571</v>
       </c>
       <c r="B39" t="n">
-        <v>0.989934369949371</v>
+        <v>0.0100656300506288</v>
       </c>
     </row>
     <row r="40">
@@ -31909,7 +31909,7 @@
         <v>572</v>
       </c>
       <c r="B40" t="n">
-        <v>0.699678617578581</v>
+        <v>0.300321382421419</v>
       </c>
     </row>
     <row r="41">
@@ -31917,7 +31917,7 @@
         <v>573</v>
       </c>
       <c r="B41" t="n">
-        <v>0.930526661978556</v>
+        <v>0.0694733380214437</v>
       </c>
     </row>
     <row r="42">
@@ -31925,7 +31925,7 @@
         <v>574</v>
       </c>
       <c r="B42" t="n">
-        <v>0.98036101464684</v>
+        <v>0.01963898535316</v>
       </c>
     </row>
     <row r="43">
@@ -31933,7 +31933,7 @@
         <v>575</v>
       </c>
       <c r="B43" t="n">
-        <v>0.991350507804869</v>
+        <v>0.00864949219513111</v>
       </c>
     </row>
     <row r="44">
@@ -31941,7 +31941,7 @@
         <v>576</v>
       </c>
       <c r="B44" t="n">
-        <v>0.893327511891778</v>
+        <v>0.106672488108222</v>
       </c>
     </row>
     <row r="45">
@@ -31949,7 +31949,7 @@
         <v>577</v>
       </c>
       <c r="B45" t="n">
-        <v>0.960407768221111</v>
+        <v>0.0395922317788887</v>
       </c>
     </row>
     <row r="46">
@@ -31957,7 +31957,7 @@
         <v>578</v>
       </c>
       <c r="B46" t="n">
-        <v>0.965821591138602</v>
+        <v>0.0341784088613979</v>
       </c>
     </row>
     <row r="47">
@@ -31965,7 +31965,7 @@
         <v>579</v>
       </c>
       <c r="B47" t="n">
-        <v>0.988274139739495</v>
+        <v>0.0117258602605047</v>
       </c>
     </row>
     <row r="48">
@@ -31973,7 +31973,7 @@
         <v>580</v>
       </c>
       <c r="B48" t="n">
-        <v>0.910975002172044</v>
+        <v>0.0890249978279556</v>
       </c>
     </row>
     <row r="49">
@@ -31981,7 +31981,7 @@
         <v>581</v>
       </c>
       <c r="B49" t="n">
-        <v>0.967680576156747</v>
+        <v>0.0323194238432528</v>
       </c>
     </row>
     <row r="50">
@@ -31989,7 +31989,7 @@
         <v>582</v>
       </c>
       <c r="B50" t="n">
-        <v>0.732248598704363</v>
+        <v>0.267751401295637</v>
       </c>
     </row>
     <row r="51">
@@ -31997,7 +31997,7 @@
         <v>583</v>
       </c>
       <c r="B51" t="n">
-        <v>0.956539361946471</v>
+        <v>0.043460638053529</v>
       </c>
     </row>
     <row r="52">
@@ -32005,7 +32005,7 @@
         <v>584</v>
       </c>
       <c r="B52" t="n">
-        <v>0.94159748026655</v>
+        <v>0.0584025197334498</v>
       </c>
     </row>
     <row r="53">
@@ -32013,7 +32013,7 @@
         <v>585</v>
       </c>
       <c r="B53" t="n">
-        <v>0.952510939183878</v>
+        <v>0.0474890608161219</v>
       </c>
     </row>
     <row r="54">
@@ -32021,7 +32021,7 @@
         <v>586</v>
       </c>
       <c r="B54" t="n">
-        <v>0.963962165699396</v>
+        <v>0.0360378343006043</v>
       </c>
     </row>
     <row r="55">
@@ -32029,7 +32029,7 @@
         <v>587</v>
       </c>
       <c r="B55" t="n">
-        <v>0.946575897825466</v>
+        <v>0.0534241021745342</v>
       </c>
     </row>
     <row r="56">
@@ -32037,7 +32037,7 @@
         <v>588</v>
       </c>
       <c r="B56" t="n">
-        <v>0.99082474966629</v>
+        <v>0.00917525033370969</v>
       </c>
     </row>
     <row r="57">
@@ -32045,7 +32045,7 @@
         <v>589</v>
       </c>
       <c r="B57" t="n">
-        <v>0.971156253218131</v>
+        <v>0.0288437467818694</v>
       </c>
     </row>
     <row r="58">
@@ -32053,7 +32053,7 @@
         <v>590</v>
       </c>
       <c r="B58" t="n">
-        <v>0.920904364151772</v>
+        <v>0.0790956358482275</v>
       </c>
     </row>
     <row r="59">
@@ -32061,7 +32061,7 @@
         <v>591</v>
       </c>
       <c r="B59" t="n">
-        <v>0.990462877631054</v>
+        <v>0.00953712236894555</v>
       </c>
     </row>
     <row r="60">
@@ -32069,7 +32069,7 @@
         <v>592</v>
       </c>
       <c r="B60" t="n">
-        <v>0.981174308084393</v>
+        <v>0.018825691915607</v>
       </c>
     </row>
     <row r="61">
@@ -32077,7 +32077,7 @@
         <v>593</v>
       </c>
       <c r="B61" t="n">
-        <v>0.870882093329359</v>
+        <v>0.129117906670641</v>
       </c>
     </row>
     <row r="62">
@@ -32085,7 +32085,7 @@
         <v>594</v>
       </c>
       <c r="B62" t="n">
-        <v>0.931274659960116</v>
+        <v>0.0687253400398844</v>
       </c>
     </row>
     <row r="63">
@@ -32093,7 +32093,7 @@
         <v>595</v>
       </c>
       <c r="B63" t="n">
-        <v>0.876740400791255</v>
+        <v>0.123259599208745</v>
       </c>
     </row>
     <row r="64">
@@ -32101,7 +32101,7 @@
         <v>596</v>
       </c>
       <c r="B64" t="n">
-        <v>0.691059997593696</v>
+        <v>0.308940002406304</v>
       </c>
     </row>
     <row r="65">
@@ -32109,7 +32109,7 @@
         <v>597</v>
       </c>
       <c r="B65" t="n">
-        <v>0.94025306564315</v>
+        <v>0.0597469343568503</v>
       </c>
     </row>
     <row r="66">
@@ -32117,7 +32117,7 @@
         <v>598</v>
       </c>
       <c r="B66" t="n">
-        <v>0.894689126609618</v>
+        <v>0.105310873390382</v>
       </c>
     </row>
   </sheetData>

</xml_diff>